<commit_message>
Se agrega la función de calendario al registrar la fecha, tambien se actualizó las entradas del formulario
</commit_message>
<xml_diff>
--- a/GestionFormulario2/src/main/resources/Formulario.xlsx
+++ b/GestionFormulario2/src/main/resources/Formulario.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">Nombre del aprendiz:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Tipo de visitante:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apellidos:</t>
   </si>
   <si>
     <t xml:space="preserve">Tipo de documento:</t>
@@ -100,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -124,6 +130,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -155,25 +168,41 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -366,65 +395,102 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>